<commit_message>
Adding 50 MeV simulated unfold
</commit_message>
<xml_diff>
--- a/Simulated/Activation/50MeVTa/50MeVTaFoils.xlsx
+++ b/Simulated/Activation/50MeVTa/50MeVTaFoils.xlsx
@@ -542,7 +542,7 @@
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -667,7 +667,7 @@
         <v>1</v>
       </c>
       <c r="P2" s="13">
-        <f>3.141592654*K2^2*L2</f>
+        <f t="shared" ref="P2:P8" si="0">3.141592654*K2^2*L2</f>
         <v>1.9634954087500001</v>
       </c>
       <c r="Q2" s="14">
@@ -675,7 +675,7 @@
         <v>567.48</v>
       </c>
       <c r="R2" s="15">
-        <f>0.6931471806/Q2</f>
+        <f t="shared" ref="R2:R8" si="1">0.6931471806/Q2</f>
         <v>1.221447770141679E-3</v>
       </c>
     </row>
@@ -726,7 +726,7 @@
         <v>0.95709999999999995</v>
       </c>
       <c r="P3" s="13">
-        <f>3.141592654*K3^2*L3</f>
+        <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
       <c r="Q3" s="14">
@@ -734,7 +734,7 @@
         <v>16200</v>
       </c>
       <c r="R3" s="15">
-        <f>0.6931471806/Q3</f>
+        <f t="shared" si="1"/>
         <v>4.2786863000000001E-5</v>
       </c>
     </row>
@@ -785,7 +785,7 @@
         <v>0.95709999999999995</v>
       </c>
       <c r="P4" s="13">
-        <f>3.141592654*K4^2*L4</f>
+        <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
       <c r="Q4" s="14">
@@ -793,7 +793,7 @@
         <v>16200</v>
       </c>
       <c r="R4" s="15">
-        <f>0.6931471806/Q4</f>
+        <f t="shared" si="1"/>
         <v>4.2786863000000001E-5</v>
       </c>
     </row>
@@ -844,7 +844,7 @@
         <v>1</v>
       </c>
       <c r="P5" s="13">
-        <f>3.141592654*K5^2*L5</f>
+        <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
       <c r="Q5" s="14">
@@ -852,7 +852,7 @@
         <v>54000</v>
       </c>
       <c r="R5" s="15">
-        <f>0.6931471806/Q5</f>
+        <f t="shared" si="1"/>
         <v>1.28360589E-5</v>
       </c>
     </row>
@@ -903,7 +903,7 @@
         <v>1</v>
       </c>
       <c r="P6" s="13">
-        <f>3.141592654*K6^2*L6</f>
+        <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
       <c r="Q6" s="14">
@@ -911,7 +911,7 @@
         <v>54000</v>
       </c>
       <c r="R6" s="15">
-        <f>0.6931471806/Q6</f>
+        <f t="shared" si="1"/>
         <v>1.28360589E-5</v>
       </c>
     </row>
@@ -962,7 +962,7 @@
         <v>0.51449999999999996</v>
       </c>
       <c r="P7" s="13">
-        <f>3.141592654*K7^2*L7</f>
+        <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
       <c r="Q7" s="14">
@@ -970,7 +970,7 @@
         <v>282276</v>
       </c>
       <c r="R7" s="15">
-        <f>0.6931471806/Q7</f>
+        <f t="shared" si="1"/>
         <v>2.4555654061981891E-6</v>
       </c>
     </row>
@@ -1021,7 +1021,7 @@
         <v>0.51449999999999996</v>
       </c>
       <c r="P8" s="13">
-        <f>3.141592654*K8^2*L8</f>
+        <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
       <c r="Q8" s="14">
@@ -1029,7 +1029,7 @@
         <v>282276</v>
       </c>
       <c r="R8" s="15">
-        <f>0.6931471806/Q8</f>
+        <f t="shared" si="1"/>
         <v>2.4555654061981891E-6</v>
       </c>
     </row>
@@ -1044,7 +1044,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="16">
-        <v>1378</v>
+        <v>1377.63</v>
       </c>
       <c r="E9" s="16">
         <v>81.7</v>
@@ -1080,7 +1080,7 @@
         <v>0.68076899999999996</v>
       </c>
       <c r="P9" s="13">
-        <f t="shared" ref="P9" si="0">3.141592654*K9^2*L9</f>
+        <f t="shared" ref="P9" si="2">3.141592654*K9^2*L9</f>
         <v>1.9634954087500001</v>
       </c>
       <c r="Q9" s="19">
@@ -1088,7 +1088,7 @@
         <v>128160</v>
       </c>
       <c r="R9" s="15">
-        <f t="shared" ref="R9" si="1">0.6931471806/Q9</f>
+        <f t="shared" ref="R9" si="3">0.6931471806/Q9</f>
         <v>5.4084517837078655E-6</v>
       </c>
     </row>

</xml_diff>